<commit_message>
Face Recognition added :octocat:
</commit_message>
<xml_diff>
--- a/symbiote/employee_assign/100000/24-04-2023.xlsx
+++ b/symbiote/employee_assign/100000/24-04-2023.xlsx
@@ -331,7 +331,7 @@
         <v>6</v>
       </c>
       <c r="E2" s="1" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="3">
@@ -348,7 +348,7 @@
         <v>6</v>
       </c>
       <c r="E3" s="1" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="4">
@@ -365,7 +365,7 @@
         <v>9</v>
       </c>
       <c r="E4" s="1" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="5">
@@ -382,7 +382,7 @@
         <v>6</v>
       </c>
       <c r="E5" s="1" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>